<commit_message>
update 2020/04/05 update Login
</commit_message>
<xml_diff>
--- a/doc/Matrix-SSM 异步流程.xlsx
+++ b/doc/Matrix-SSM 异步流程.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyWork\learnspace\my-github\matrix-ssm\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1E2603-AF85-45F4-A750-95D7A225A161}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31104C1F-3BA8-45FC-8DFB-64F588B254CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="异步处理" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="RuoYi异步处理结构" sheetId="2" r:id="rId1"/>
+    <sheet name="Java线程池-ThreadPoolExecutor" sheetId="4" r:id="rId2"/>
+    <sheet name="Spring-ThreadPoolTaskExecutor" sheetId="3" r:id="rId3"/>
+    <sheet name="二者区别" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,9 +27,40 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>参考文章</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.ideabuffer.cn/2017/04/04/%E6%B7%B1%E5%85%A5%E7%90%86%E8%A7%A3Java%E7%BA%BF%E7%A8%8B%E6%B1%A0%EF%BC%9AThreadPoolExecutor/#addWorker%E6%96%B9%E6%B3%95</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.jianshu.com/p/502f9952c09b</t>
+  </si>
+  <si>
+    <t>ScheduledThreadPoolExecutor结构</t>
+  </si>
+  <si>
+    <t>https://www.jianshu.com/p/125ccf0046f3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://ifeve.com/java-threadpool/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.jianshu.com/p/3561d925816f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,6 +73,14 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -60,14 +101,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1101,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35415AF7-6E98-4100-A7EC-6256CE7CBF5F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1115,14 +1159,93 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7E9A4F-3696-45D7-A364-2E22139F5906}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" location="addWorker%E6%96%B9%E6%B3%95" xr:uid="{E3CAA2D6-64DC-4415-BE28-7DC21446CEB4}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{53ABD8E0-AECC-403B-8A40-ACE36A1FAAE7}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{EB9C81CD-592E-4B62-9E83-A35F16D46CAA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06854A2A-F2CF-41AB-88A7-CB9FA9D390A6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2913C1-23D5-41A3-BA9C-75405833CA89}">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{C01676F4-B129-4664-95DC-511E6F12AC10}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>